<commit_message>
rounded colunns in package source & made toi_source categorical
</commit_message>
<xml_diff>
--- a/eims-toi-transect/bottleEn617withoutincubation.xlsx
+++ b/eims-toi-transect/bottleEn617withoutincubation.xlsx
@@ -74,9 +74,6 @@
     <t>toi_source</t>
   </si>
   <si>
-    <t>character</t>
-  </si>
-  <si>
     <t>niskin</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t xml:space="preserve">Depth of sample below sea surface  </t>
+  </si>
+  <si>
+    <t>categorical</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -553,7 +553,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -581,30 +581,30 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
         <v>39</v>
       </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -612,18 +612,18 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -632,18 +632,18 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -652,46 +652,46 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -702,10 +702,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -716,10 +716,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -730,10 +730,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -744,10 +744,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>

</xml_diff>